<commit_message>
Added connection to transaction log
</commit_message>
<xml_diff>
--- a/eg-pos-mortem/reports/MPUL-20220413000000-20220413235959.xlsx
+++ b/eg-pos-mortem/reports/MPUL-20220413000000-20220413235959.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="201">
   <si>
     <t>Autor</t>
   </si>
@@ -1002,7 +1002,7 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:50:49.630</t>
+    <t/>
   </si>
   <si>
     <t>9991200600007718</t>
@@ -1015,6 +1015,9 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>Checkin,ECommNoSeguro</t>
   </si>
   <si>
@@ -1022,9 +1025,6 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:52:49.909</t>
-  </si>
-  <si>
     <t>9752220600007715</t>
   </si>
   <si>
@@ -1039,42 +1039,15 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:52:50.610</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][null][MR]
 INCORRECTO:[igual][0220][0200]</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>CardOnFile,Compra</t>
   </si>
   <si>
     <t>CardOnFile:existe(acq.req.63.PJ)
 Compra:igual(acq.req.mti,0200) y igual(acq.req.3,000000) y no existe(acq.req.39)</t>
-  </si>
-  <si>
-    <t>18:52:51.249</t>
-  </si>
-  <si>
-    <t>18:52:52.200</t>
-  </si>
-  <si>
-    <t>18:52:53.430</t>
-  </si>
-  <si>
-    <t>18:52:54.623</t>
-  </si>
-  <si>
-    <t>18:52:55.542</t>
-  </si>
-  <si>
-    <t>18:52:56.701</t>
-  </si>
-  <si>
-    <t>18:52:57.371</t>
   </si>
   <si>
     <t>Reverso,CardOnFile,ECommNoSeguro</t>
@@ -1085,19 +1058,10 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:52:58.022</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][MC][MR]
 INCORRECTO:[igual][0420][0200]</t>
   </si>
   <si>
-    <t>18:53:01.990</t>
-  </si>
-  <si>
-    <t>18:53:14.570</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][ER][MR]
 CORRECTO</t>
   </si>
@@ -1109,41 +1073,14 @@
 VerificacionCuenta:igual(acq.req.mti,0200) y igual(acq.req.3,810000)</t>
   </si>
   <si>
-    <t>18:53:21.708</t>
-  </si>
-  <si>
-    <t>18:53:28.799</t>
-  </si>
-  <si>
-    <t>18:53:33.499</t>
-  </si>
-  <si>
-    <t>18:53:38.408</t>
-  </si>
-  <si>
-    <t>18:53:45.638</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][C ][MR]
 CORRECTO</t>
   </si>
   <si>
-    <t>18:53:52.739</t>
-  </si>
-  <si>
-    <t>18:53:57.307</t>
-  </si>
-  <si>
-    <t>18:54:03.629</t>
-  </si>
-  <si>
     <t>CORRECTO
 CORRECTO</t>
   </si>
   <si>
-    <t>18:54:11.731</t>
-  </si>
-  <si>
     <t>Compra,ECommNoSeguro</t>
   </si>
   <si>
@@ -1151,26 +1088,14 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:54:19.589</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][null][MR]
 CORRECTO</t>
   </si>
   <si>
-    <t>18:54:26.608</t>
-  </si>
-  <si>
-    <t>18:54:36.738</t>
-  </si>
-  <si>
     <t>Compra</t>
   </si>
   <si>
     <t>Compra:igual(acq.req.mti,0200) y igual(acq.req.3,000000) y no existe(acq.req.39)</t>
-  </si>
-  <si>
-    <t>18:54:44.047</t>
   </si>
   <si>
     <t>TarjetaPresente,Compra</t>
@@ -1180,31 +1105,10 @@
 Compra:igual(acq.req.mti,0200) y igual(acq.req.3,000000) y no existe(acq.req.39)</t>
   </si>
   <si>
-    <t>18:54:49.330</t>
-  </si>
-  <si>
-    <t>18:54:56.908</t>
-  </si>
-  <si>
-    <t>18:55:01.548</t>
-  </si>
-  <si>
-    <t>18:55:06.816</t>
-  </si>
-  <si>
     <t>Devolucion</t>
   </si>
   <si>
     <t>Devolucion:igual(acq.req.mti,0200) y igual(acq.req.3,200000)</t>
-  </si>
-  <si>
-    <t>18:55:13.937</t>
-  </si>
-  <si>
-    <t>18:55:18.846</t>
-  </si>
-  <si>
-    <t>18:55:25.887</t>
   </si>
   <si>
     <t>Reverso,ECommNoSeguro</t>
@@ -1214,22 +1118,10 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:55:33.299</t>
-  </si>
-  <si>
     <t>INCORRECTO:[igual][null][MR]
 INCORRECTO:[igual][0420][0200]</t>
   </si>
   <si>
-    <t>18:55:42.268</t>
-  </si>
-  <si>
-    <t>18:55:49.518</t>
-  </si>
-  <si>
-    <t>18:55:56.648</t>
-  </si>
-  <si>
     <t>Reverso,TarjetaPresente</t>
   </si>
   <si>
@@ -1237,92 +1129,14 @@
 TarjetaPresente:igual(acq.req.22.1,[05, 07, 80, 90, 91])</t>
   </si>
   <si>
-    <t>18:56:01.299</t>
-  </si>
-  <si>
-    <t>18:56:06.488</t>
-  </si>
-  <si>
-    <t>18:56:11.890</t>
-  </si>
-  <si>
-    <t>18:56:17.746</t>
-  </si>
-  <si>
-    <t>18:56:22.887</t>
-  </si>
-  <si>
-    <t>18:56:30.707</t>
-  </si>
-  <si>
-    <t>18:56:36.108</t>
-  </si>
-  <si>
-    <t>18:56:41.528</t>
-  </si>
-  <si>
-    <t>18:56:46.950</t>
-  </si>
-  <si>
-    <t>18:56:54.498</t>
-  </si>
-  <si>
-    <t>18:56:59.446</t>
-  </si>
-  <si>
     <t>9966510899032610</t>
-  </si>
-  <si>
-    <t>18:57:07.387</t>
-  </si>
-  <si>
-    <t>18:57:13.637</t>
-  </si>
-  <si>
-    <t>18:57:26.417</t>
   </si>
   <si>
     <t>INCORRECTO:[igual][EC][MR]
 CORRECTO</t>
   </si>
   <si>
-    <t>18:57:35.987</t>
-  </si>
-  <si>
-    <t>18:57:43.256</t>
-  </si>
-  <si>
-    <t>18:57:52.037</t>
-  </si>
-  <si>
-    <t>18:57:59.427</t>
-  </si>
-  <si>
-    <t>18:58:06.388</t>
-  </si>
-  <si>
-    <t>18:58:13.118</t>
-  </si>
-  <si>
-    <t>18:58:22.109</t>
-  </si>
-  <si>
-    <t>18:58:29.408</t>
-  </si>
-  <si>
-    <t>18:58:34.619</t>
-  </si>
-  <si>
     <t>9752283899032612</t>
-  </si>
-  <si>
-    <t>18:58:39.658</t>
-  </si>
-  <si>
-    <t>18:58:44.388</t>
-  </si>
-  <si>
-    <t>18:58:52.037</t>
   </si>
   <si>
     <t>Devolucion,ECommNoSeguro</t>
@@ -1332,9 +1146,6 @@
 ECommNoSeguro:igual(acq.req.63.C0.5,[5, 6]) y igual(acq.req.63.Q2,09) y igual(acq.req.25,59) y igual(acq.req.22.1,[01, 10])</t>
   </si>
   <si>
-    <t>18:58:57.097</t>
-  </si>
-  <si>
     <t>Promocion,Checkin</t>
   </si>
   <si>
@@ -1342,275 +1153,35 @@
 Checkin:igual(acq.req.mti,0100) y igual(acq.req.3,000000)</t>
   </si>
   <si>
-    <t>18:59:01.956</t>
-  </si>
-  <si>
     <t>9752243899032616</t>
   </si>
   <si>
-    <t>18:59:06.439</t>
-  </si>
-  <si>
-    <t>18:59:13.678</t>
-  </si>
-  <si>
-    <t>18:59:24.899</t>
-  </si>
-  <si>
-    <t>18:59:29.738</t>
-  </si>
-  <si>
-    <t>18:59:34.450</t>
-  </si>
-  <si>
-    <t>18:59:39.259</t>
-  </si>
-  <si>
-    <t>18:59:44.006</t>
-  </si>
-  <si>
-    <t>18:59:49.158</t>
-  </si>
-  <si>
-    <t>18:59:54.154</t>
-  </si>
-  <si>
-    <t>18:59:58.808</t>
-  </si>
-  <si>
     <t>iap_BBVA_PE_ADQ_TPV_B1_01</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>19:00:05.920</t>
-  </si>
-  <si>
     <t>9752205900000007</t>
   </si>
   <si>
-    <t>19:00:06.550</t>
-  </si>
-  <si>
     <t>Compra:igual(acq.req.mti,0200) y igual(acq.req.3,000000)</t>
   </si>
   <si>
-    <t>19:00:07.660</t>
-  </si>
-  <si>
     <t>9752205900000023</t>
-  </si>
-  <si>
-    <t>19:00:08.305</t>
-  </si>
-  <si>
-    <t>19:00:09.785</t>
-  </si>
-  <si>
-    <t>19:00:10.243</t>
-  </si>
-  <si>
-    <t>19:00:10.876</t>
-  </si>
-  <si>
-    <t>19:00:11.487</t>
   </si>
   <si>
     <t>INCORRECTO:[igual][null][MR]
 INCORRECTO:[igual][0400][0200]</t>
   </si>
   <si>
-    <t>19:00:11.878</t>
-  </si>
-  <si>
-    <t>19:00:12.321</t>
-  </si>
-  <si>
     <t>iap_BBVA_PE_ADQ_INT_REDSYS_B1_01</t>
   </si>
   <si>
-    <t>19:21:42.089</t>
-  </si>
-  <si>
-    <t>19:23:12.959</t>
-  </si>
-  <si>
-    <t>19:23:13.177</t>
-  </si>
-  <si>
-    <t>19:23:14.126</t>
-  </si>
-  <si>
-    <t>19:24:23.987</t>
-  </si>
-  <si>
-    <t>19:24:50.806</t>
-  </si>
-  <si>
-    <t>19:24:51.027</t>
-  </si>
-  <si>
-    <t>19:25:06.817</t>
-  </si>
-  <si>
-    <t>19:25:07.269</t>
-  </si>
-  <si>
-    <t>19:26:14.695</t>
-  </si>
-  <si>
-    <t>19:26:14.896</t>
-  </si>
-  <si>
-    <t>19:30:52.687</t>
-  </si>
-  <si>
-    <t>19:30:53.107</t>
-  </si>
-  <si>
-    <t>19:30:53.665</t>
-  </si>
-  <si>
-    <t>19:30:54.086</t>
-  </si>
-  <si>
-    <t>19:30:55.416</t>
-  </si>
-  <si>
-    <t>19:30:56.177</t>
-  </si>
-  <si>
-    <t>19:30:56.758</t>
-  </si>
-  <si>
-    <t>19:30:57.367</t>
-  </si>
-  <si>
-    <t>19:30:57.929</t>
-  </si>
-  <si>
-    <t>19:30:58.267</t>
-  </si>
-  <si>
-    <t>19:30:58.988</t>
-  </si>
-  <si>
-    <t>19:30:59.898</t>
-  </si>
-  <si>
-    <t>19:31:01.098</t>
-  </si>
-  <si>
-    <t>19:31:02.586</t>
-  </si>
-  <si>
-    <t>19:31:08.477</t>
-  </si>
-  <si>
-    <t>19:31:20.867</t>
-  </si>
-  <si>
-    <t>19:31:27.188</t>
-  </si>
-  <si>
-    <t>19:31:35.027</t>
-  </si>
-  <si>
-    <t>19:31:42.388</t>
-  </si>
-  <si>
-    <t>19:31:43.197</t>
-  </si>
-  <si>
-    <t>19:35:37.956</t>
-  </si>
-  <si>
-    <t>19:35:38.476</t>
-  </si>
-  <si>
-    <t>19:35:46.327</t>
-  </si>
-  <si>
-    <t>19:35:46.627</t>
-  </si>
-  <si>
-    <t>19:36:04.498</t>
-  </si>
-  <si>
-    <t>19:36:04.889</t>
-  </si>
-  <si>
-    <t>19:36:15.497</t>
-  </si>
-  <si>
-    <t>19:36:16.077</t>
-  </si>
-  <si>
-    <t>19:36:23.826</t>
-  </si>
-  <si>
-    <t>19:36:29.417</t>
-  </si>
-  <si>
-    <t>19:38:53.106</t>
-  </si>
-  <si>
-    <t>19:40:21.998</t>
-  </si>
-  <si>
-    <t>19:40:26.707</t>
-  </si>
-  <si>
-    <t>19:40:42.967</t>
-  </si>
-  <si>
-    <t>19:40:59.885</t>
-  </si>
-  <si>
-    <t>19:41:18.566</t>
-  </si>
-  <si>
-    <t>19:41:53.535</t>
-  </si>
-  <si>
-    <t>19:42:52.526</t>
-  </si>
-  <si>
-    <t>19:44:36.405</t>
-  </si>
-  <si>
     <t>Checkin</t>
   </si>
   <si>
     <t>Checkin:igual(acq.req.mti,0100) y igual(acq.req.3,000000)</t>
   </si>
   <si>
-    <t>19:45:51.716</t>
-  </si>
-  <si>
-    <t>19:46:19.509</t>
-  </si>
-  <si>
-    <t>19:46:19.897</t>
-  </si>
-  <si>
-    <t>19:46:35.177</t>
-  </si>
-  <si>
-    <t>19:46:35.567</t>
-  </si>
-  <si>
-    <t>19:46:52.005</t>
-  </si>
-  <si>
-    <t>19:46:52.406</t>
-  </si>
-  <si>
-    <t>19:47:10.791</t>
-  </si>
-  <si>
-    <t>19:55:10.088</t>
+    <t>2022-04-13 19:55:10.080</t>
   </si>
 </sst>
 </file>
@@ -5503,13 +5074,13 @@
         <v>145</v>
       </c>
       <c r="J18" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="K18" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="L18" t="s">
-        <v>343</v>
+        <v>200</v>
       </c>
       <c r="M18" t="s">
         <v>149</v>
@@ -5518,7 +5089,7 @@
         <v>143</v>
       </c>
       <c r="O18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P18"/>
       <c r="Q18" t="s">
@@ -5572,13 +5143,13 @@
         <v>124</v>
       </c>
       <c r="AK18" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="AL18" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN18" s="18" t="str">
         <f t="shared" ref="AN18:AN81" si="0"><![CDATA[IF(OR(
@@ -5625,7 +5196,7 @@
         <v>158</v>
       </c>
       <c r="L19" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="M19" t="s">
         <v>155</v>
@@ -5634,7 +5205,7 @@
         <v>134</v>
       </c>
       <c r="O19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P19"/>
       <c r="Q19" t="s">
@@ -5664,7 +5235,7 @@
         <v>124</v>
       </c>
       <c r="AC19" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD19" s="18" t="s">
         <v>124</v>
@@ -5676,7 +5247,7 @@
         <v>124</v>
       </c>
       <c r="AG19" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH19" s="18" t="s">
         <v>124</v>
@@ -5688,7 +5259,7 @@
         <v>124</v>
       </c>
       <c r="AK19" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL19" s="18" t="s">
         <v>124</v>
@@ -5721,13 +5292,13 @@
         <v>145</v>
       </c>
       <c r="J20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="M20" t="s">
         <v>149</v>
@@ -5766,31 +5337,31 @@
         <v>124</v>
       </c>
       <c r="AC20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD20" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF20" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH20" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI20" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ20" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK20" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL20" s="18" t="s">
         <v>124</v>
@@ -5829,7 +5400,7 @@
         <v>147</v>
       </c>
       <c r="L21" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="M21" t="s">
         <v>149</v>
@@ -5892,7 +5463,7 @@
         <v>124</v>
       </c>
       <c r="AK21" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL21" s="18" t="s">
         <v>124</v>
@@ -5931,7 +5502,7 @@
         <v>147</v>
       </c>
       <c r="L22" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="M22" t="s">
         <v>149</v>
@@ -5994,7 +5565,7 @@
         <v>124</v>
       </c>
       <c r="AK22" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL22" s="18" t="s">
         <v>124</v>
@@ -6033,7 +5604,7 @@
         <v>147</v>
       </c>
       <c r="L23" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="M23" t="s">
         <v>149</v>
@@ -6096,7 +5667,7 @@
         <v>124</v>
       </c>
       <c r="AK23" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL23" s="18" t="s">
         <v>124</v>
@@ -6135,7 +5706,7 @@
         <v>147</v>
       </c>
       <c r="L24" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="M24" t="s">
         <v>149</v>
@@ -6198,7 +5769,7 @@
         <v>124</v>
       </c>
       <c r="AK24" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL24" s="18" t="s">
         <v>124</v>
@@ -6237,7 +5808,7 @@
         <v>147</v>
       </c>
       <c r="L25" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="M25" t="s">
         <v>149</v>
@@ -6300,7 +5871,7 @@
         <v>124</v>
       </c>
       <c r="AK25" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL25" s="18" t="s">
         <v>124</v>
@@ -6339,7 +5910,7 @@
         <v>147</v>
       </c>
       <c r="L26" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="M26" t="s">
         <v>149</v>
@@ -6402,7 +5973,7 @@
         <v>124</v>
       </c>
       <c r="AK26" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL26" s="18" t="s">
         <v>124</v>
@@ -6435,13 +6006,13 @@
         <v>145</v>
       </c>
       <c r="J27" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="K27" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="L27" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="M27" t="s">
         <v>149</v>
@@ -6450,7 +6021,7 @@
         <v>134</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="P27"/>
       <c r="Q27" s="18" t="s">
@@ -6480,7 +6051,7 @@
         <v>124</v>
       </c>
       <c r="AC27" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD27" s="18" t="s">
         <v>124</v>
@@ -6492,7 +6063,7 @@
         <v>124</v>
       </c>
       <c r="AG27" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH27" s="18" t="s">
         <v>124</v>
@@ -6504,7 +6075,7 @@
         <v>124</v>
       </c>
       <c r="AK27" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL27" s="18" t="s">
         <v>124</v>
@@ -6543,7 +6114,7 @@
         <v>147</v>
       </c>
       <c r="L28" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="M28" t="s">
         <v>149</v>
@@ -6606,7 +6177,7 @@
         <v>124</v>
       </c>
       <c r="AK28" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL28" s="18" t="s">
         <v>124</v>
@@ -6639,13 +6210,13 @@
         <v>145</v>
       </c>
       <c r="J29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L29" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="M29" t="s">
         <v>149</v>
@@ -6654,7 +6225,7 @@
         <v>134</v>
       </c>
       <c r="O29" s="18" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="P29"/>
       <c r="Q29" s="18" t="s">
@@ -6690,7 +6261,7 @@
         <v>124</v>
       </c>
       <c r="AE29" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF29" s="18" t="s">
         <v>124</v>
@@ -6708,7 +6279,7 @@
         <v>124</v>
       </c>
       <c r="AK29" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL29" s="18" t="s">
         <v>124</v>
@@ -6741,13 +6312,13 @@
         <v>145</v>
       </c>
       <c r="J30" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="K30" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="L30" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="M30" t="s">
         <v>149</v>
@@ -6756,7 +6327,7 @@
         <v>134</v>
       </c>
       <c r="O30" s="18" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="P30"/>
       <c r="Q30" s="18" t="s">
@@ -6792,7 +6363,7 @@
         <v>124</v>
       </c>
       <c r="AE30" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF30" s="18" t="s">
         <v>124</v>
@@ -6810,7 +6381,7 @@
         <v>124</v>
       </c>
       <c r="AK30" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL30" s="18" t="s">
         <v>124</v>
@@ -6843,13 +6414,13 @@
         <v>145</v>
       </c>
       <c r="J31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L31" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="M31" t="s">
         <v>149</v>
@@ -6858,7 +6429,7 @@
         <v>134</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="P31"/>
       <c r="Q31" s="18" t="s">
@@ -6912,7 +6483,7 @@
         <v>124</v>
       </c>
       <c r="AK31" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL31" s="18" t="s">
         <v>124</v>
@@ -6945,13 +6516,13 @@
         <v>145</v>
       </c>
       <c r="J32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L32" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="M32" t="s">
         <v>149</v>
@@ -6990,31 +6561,31 @@
         <v>124</v>
       </c>
       <c r="AC32" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD32" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE32" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF32" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG32" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH32" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI32" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ32" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK32" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL32" s="18" t="s">
         <v>124</v>
@@ -7047,13 +6618,13 @@
         <v>145</v>
       </c>
       <c r="J33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L33" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="M33" t="s">
         <v>149</v>
@@ -7092,31 +6663,31 @@
         <v>124</v>
       </c>
       <c r="AC33" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD33" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE33" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF33" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG33" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH33" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI33" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ33" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK33" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL33" s="18" t="s">
         <v>124</v>
@@ -7149,13 +6720,13 @@
         <v>145</v>
       </c>
       <c r="J34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L34" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="M34" t="s">
         <v>149</v>
@@ -7164,7 +6735,7 @@
         <v>134</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="P34"/>
       <c r="Q34" s="18" t="s">
@@ -7218,7 +6789,7 @@
         <v>124</v>
       </c>
       <c r="AK34" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL34" s="18" t="s">
         <v>124</v>
@@ -7251,13 +6822,13 @@
         <v>145</v>
       </c>
       <c r="J35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L35" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="M35" t="s">
         <v>149</v>
@@ -7266,7 +6837,7 @@
         <v>134</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="P35"/>
       <c r="Q35" s="18" t="s">
@@ -7296,31 +6867,31 @@
         <v>124</v>
       </c>
       <c r="AC35" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD35" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE35" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF35" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG35" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH35" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI35" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ35" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK35" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL35" s="18" t="s">
         <v>124</v>
@@ -7353,13 +6924,13 @@
         <v>145</v>
       </c>
       <c r="J36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L36" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="M36" t="s">
         <v>149</v>
@@ -7398,31 +6969,31 @@
         <v>124</v>
       </c>
       <c r="AC36" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD36" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE36" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF36" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG36" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH36" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI36" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ36" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK36" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL36" s="18" t="s">
         <v>124</v>
@@ -7455,13 +7026,13 @@
         <v>145</v>
       </c>
       <c r="J37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K37" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L37" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="M37" t="s">
         <v>149</v>
@@ -7470,7 +7041,7 @@
         <v>134</v>
       </c>
       <c r="O37" s="18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="P37"/>
       <c r="Q37" s="18" t="s">
@@ -7506,7 +7077,7 @@
         <v>124</v>
       </c>
       <c r="AE37" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF37" s="18" t="s">
         <v>124</v>
@@ -7524,7 +7095,7 @@
         <v>124</v>
       </c>
       <c r="AK37" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL37" s="18" t="s">
         <v>124</v>
@@ -7557,13 +7128,13 @@
         <v>145</v>
       </c>
       <c r="J38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L38" t="s">
-        <v>190</v>
+        <v>148</v>
       </c>
       <c r="M38" t="s">
         <v>149</v>
@@ -7572,7 +7143,7 @@
         <v>134</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="P38"/>
       <c r="Q38" s="18" t="s">
@@ -7608,7 +7179,7 @@
         <v>124</v>
       </c>
       <c r="AE38" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF38" s="18" t="s">
         <v>124</v>
@@ -7626,7 +7197,7 @@
         <v>124</v>
       </c>
       <c r="AK38" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL38" s="18" t="s">
         <v>124</v>
@@ -7659,13 +7230,13 @@
         <v>145</v>
       </c>
       <c r="J39" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="K39" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="L39" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="M39" t="s">
         <v>149</v>
@@ -7674,7 +7245,7 @@
         <v>134</v>
       </c>
       <c r="O39" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P39"/>
       <c r="Q39" s="18" t="s">
@@ -7728,7 +7299,7 @@
         <v>124</v>
       </c>
       <c r="AK39" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL39" s="18" t="s">
         <v>124</v>
@@ -7761,13 +7332,13 @@
         <v>145</v>
       </c>
       <c r="J40" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="K40" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="L40" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="M40" t="s">
         <v>149</v>
@@ -7776,7 +7347,7 @@
         <v>134</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P40"/>
       <c r="Q40" s="18" t="s">
@@ -7830,7 +7401,7 @@
         <v>124</v>
       </c>
       <c r="AK40" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL40" s="18" t="s">
         <v>124</v>
@@ -7863,13 +7434,13 @@
         <v>145</v>
       </c>
       <c r="J41" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="K41" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="L41" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="M41" t="s">
         <v>149</v>
@@ -7878,7 +7449,7 @@
         <v>134</v>
       </c>
       <c r="O41" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P41"/>
       <c r="Q41" s="18" t="s">
@@ -7932,7 +7503,7 @@
         <v>124</v>
       </c>
       <c r="AK41" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL41" s="18" t="s">
         <v>124</v>
@@ -7965,13 +7536,13 @@
         <v>145</v>
       </c>
       <c r="J42" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="K42" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="L42" t="s">
-        <v>199</v>
+        <v>148</v>
       </c>
       <c r="M42" t="s">
         <v>149</v>
@@ -7980,7 +7551,7 @@
         <v>134</v>
       </c>
       <c r="O42" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P42"/>
       <c r="Q42" s="18" t="s">
@@ -8010,31 +7581,31 @@
         <v>124</v>
       </c>
       <c r="AC42" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD42" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE42" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF42" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG42" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH42" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI42" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ42" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK42" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL42" s="18" t="s">
         <v>124</v>
@@ -8067,13 +7638,13 @@
         <v>145</v>
       </c>
       <c r="J43" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K43" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L43" t="s">
-        <v>202</v>
+        <v>148</v>
       </c>
       <c r="M43" t="s">
         <v>149</v>
@@ -8082,7 +7653,7 @@
         <v>134</v>
       </c>
       <c r="O43" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P43"/>
       <c r="Q43" s="18" t="s">
@@ -8112,31 +7683,31 @@
         <v>124</v>
       </c>
       <c r="AC43" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD43" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE43" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF43" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG43" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH43" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI43" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ43" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK43" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL43" s="18" t="s">
         <v>124</v>
@@ -8166,16 +7737,16 @@
         <v>123</v>
       </c>
       <c r="H44" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J44" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K44" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L44" t="s">
-        <v>294</v>
+        <v>148</v>
       </c>
       <c r="M44" t="s">
         <v>149</v>
@@ -8184,7 +7755,7 @@
         <v>134</v>
       </c>
       <c r="O44" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P44"/>
       <c r="Q44" s="18" t="s">
@@ -8220,7 +7791,7 @@
         <v>124</v>
       </c>
       <c r="AE44" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF44" s="18" t="s">
         <v>124</v>
@@ -8238,13 +7809,13 @@
         <v>124</v>
       </c>
       <c r="AK44" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL44" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM44" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN44" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8268,16 +7839,16 @@
         <v>123</v>
       </c>
       <c r="H45" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J45" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K45" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L45" t="s">
-        <v>295</v>
+        <v>148</v>
       </c>
       <c r="M45" t="s">
         <v>149</v>
@@ -8286,7 +7857,7 @@
         <v>134</v>
       </c>
       <c r="O45" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P45"/>
       <c r="Q45" s="18" t="s">
@@ -8322,7 +7893,7 @@
         <v>124</v>
       </c>
       <c r="AE45" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF45" s="18" t="s">
         <v>124</v>
@@ -8340,13 +7911,13 @@
         <v>124</v>
       </c>
       <c r="AK45" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL45" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM45" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN45" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8370,16 +7941,16 @@
         <v>123</v>
       </c>
       <c r="H46" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J46" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K46" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L46" t="s">
-        <v>296</v>
+        <v>148</v>
       </c>
       <c r="M46" t="s">
         <v>149</v>
@@ -8388,7 +7959,7 @@
         <v>134</v>
       </c>
       <c r="O46" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P46"/>
       <c r="Q46" s="18" t="s">
@@ -8424,7 +7995,7 @@
         <v>124</v>
       </c>
       <c r="AE46" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF46" s="18" t="s">
         <v>124</v>
@@ -8442,13 +8013,13 @@
         <v>124</v>
       </c>
       <c r="AK46" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL46" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM46" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN46" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8475,13 +8046,13 @@
         <v>145</v>
       </c>
       <c r="J47" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="K47" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="L47" t="s">
-        <v>297</v>
+        <v>148</v>
       </c>
       <c r="M47" t="s">
         <v>149</v>
@@ -8490,7 +8061,7 @@
         <v>134</v>
       </c>
       <c r="O47" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P47"/>
       <c r="Q47" s="18" t="s">
@@ -8544,13 +8115,13 @@
         <v>124</v>
       </c>
       <c r="AK47" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL47" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM47" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN47" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8577,13 +8148,13 @@
         <v>145</v>
       </c>
       <c r="J48" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="K48" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="L48" t="s">
-        <v>298</v>
+        <v>148</v>
       </c>
       <c r="M48" t="s">
         <v>149</v>
@@ -8592,7 +8163,7 @@
         <v>134</v>
       </c>
       <c r="O48" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P48"/>
       <c r="Q48" s="18" t="s">
@@ -8628,7 +8199,7 @@
         <v>124</v>
       </c>
       <c r="AE48" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF48" s="18" t="s">
         <v>124</v>
@@ -8646,13 +8217,13 @@
         <v>124</v>
       </c>
       <c r="AK48" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL48" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM48" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN48" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8676,16 +8247,16 @@
         <v>123</v>
       </c>
       <c r="H49" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J49" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="K49" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="L49" t="s">
-        <v>315</v>
+        <v>148</v>
       </c>
       <c r="M49" t="s">
         <v>149</v>
@@ -8694,7 +8265,7 @@
         <v>134</v>
       </c>
       <c r="O49" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P49"/>
       <c r="Q49" s="18" t="s">
@@ -8724,19 +8295,19 @@
         <v>124</v>
       </c>
       <c r="AC49" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD49" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE49" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF49" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG49" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH49" s="18" t="s">
         <v>124</v>
@@ -8748,13 +8319,13 @@
         <v>124</v>
       </c>
       <c r="AK49" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL49" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM49" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN49" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8778,16 +8349,16 @@
         <v>123</v>
       </c>
       <c r="H50" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J50" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="K50" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="L50" t="s">
-        <v>317</v>
+        <v>148</v>
       </c>
       <c r="M50" t="s">
         <v>149</v>
@@ -8796,7 +8367,7 @@
         <v>134</v>
       </c>
       <c r="O50" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P50"/>
       <c r="Q50" s="18" t="s">
@@ -8826,19 +8397,19 @@
         <v>124</v>
       </c>
       <c r="AC50" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD50" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE50" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF50" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG50" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH50" s="18" t="s">
         <v>124</v>
@@ -8850,13 +8421,13 @@
         <v>124</v>
       </c>
       <c r="AK50" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL50" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM50" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN50" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8880,16 +8451,16 @@
         <v>123</v>
       </c>
       <c r="H51" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J51" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K51" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L51" t="s">
-        <v>319</v>
+        <v>148</v>
       </c>
       <c r="M51" t="s">
         <v>149</v>
@@ -8898,7 +8469,7 @@
         <v>134</v>
       </c>
       <c r="O51" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P51"/>
       <c r="Q51" s="18" t="s">
@@ -8934,7 +8505,7 @@
         <v>124</v>
       </c>
       <c r="AE51" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF51" s="18" t="s">
         <v>124</v>
@@ -8952,13 +8523,13 @@
         <v>124</v>
       </c>
       <c r="AK51" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL51" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM51" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN51" s="18" t="str">
         <f t="shared" si="0"/>
@@ -8982,16 +8553,16 @@
         <v>123</v>
       </c>
       <c r="H52" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J52" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K52" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L52" t="s">
-        <v>321</v>
+        <v>148</v>
       </c>
       <c r="M52" t="s">
         <v>149</v>
@@ -9000,7 +8571,7 @@
         <v>134</v>
       </c>
       <c r="O52" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P52"/>
       <c r="Q52" s="18" t="s">
@@ -9036,7 +8607,7 @@
         <v>124</v>
       </c>
       <c r="AE52" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF52" s="18" t="s">
         <v>124</v>
@@ -9054,13 +8625,13 @@
         <v>124</v>
       </c>
       <c r="AK52" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL52" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM52" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN52" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9084,16 +8655,16 @@
         <v>123</v>
       </c>
       <c r="H53" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J53" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K53" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L53" t="s">
-        <v>323</v>
+        <v>148</v>
       </c>
       <c r="M53" t="s">
         <v>149</v>
@@ -9102,7 +8673,7 @@
         <v>134</v>
       </c>
       <c r="O53" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P53"/>
       <c r="Q53" s="18" t="s">
@@ -9138,7 +8709,7 @@
         <v>124</v>
       </c>
       <c r="AE53" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF53" s="18" t="s">
         <v>124</v>
@@ -9156,13 +8727,13 @@
         <v>124</v>
       </c>
       <c r="AK53" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL53" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM53" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN53" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9186,16 +8757,16 @@
         <v>123</v>
       </c>
       <c r="H54" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J54" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K54" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L54" t="s">
-        <v>309</v>
+        <v>148</v>
       </c>
       <c r="M54" t="s">
         <v>149</v>
@@ -9204,7 +8775,7 @@
         <v>134</v>
       </c>
       <c r="O54" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P54"/>
       <c r="Q54" s="18" t="s">
@@ -9240,7 +8811,7 @@
         <v>124</v>
       </c>
       <c r="AE54" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF54" s="18" t="s">
         <v>124</v>
@@ -9258,13 +8829,13 @@
         <v>124</v>
       </c>
       <c r="AK54" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL54" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM54" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN54" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9288,16 +8859,16 @@
         <v>123</v>
       </c>
       <c r="H55" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J55" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K55" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L55" t="s">
-        <v>310</v>
+        <v>148</v>
       </c>
       <c r="M55" t="s">
         <v>149</v>
@@ -9306,7 +8877,7 @@
         <v>134</v>
       </c>
       <c r="O55" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P55"/>
       <c r="Q55" s="18" t="s">
@@ -9342,7 +8913,7 @@
         <v>124</v>
       </c>
       <c r="AE55" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF55" s="18" t="s">
         <v>124</v>
@@ -9360,13 +8931,13 @@
         <v>124</v>
       </c>
       <c r="AK55" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL55" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM55" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN55" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9390,16 +8961,16 @@
         <v>123</v>
       </c>
       <c r="H56" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J56" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K56" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L56" t="s">
-        <v>311</v>
+        <v>148</v>
       </c>
       <c r="M56" t="s">
         <v>149</v>
@@ -9408,7 +8979,7 @@
         <v>134</v>
       </c>
       <c r="O56" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P56"/>
       <c r="Q56" s="18" t="s">
@@ -9444,31 +9015,31 @@
         <v>124</v>
       </c>
       <c r="AE56" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF56" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG56" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH56" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI56" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ56" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK56" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL56" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM56" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN56" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9492,16 +9063,16 @@
         <v>123</v>
       </c>
       <c r="H57" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J57" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K57" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L57" t="s">
-        <v>312</v>
+        <v>148</v>
       </c>
       <c r="M57" t="s">
         <v>149</v>
@@ -9510,7 +9081,7 @@
         <v>134</v>
       </c>
       <c r="O57" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P57"/>
       <c r="Q57" s="18" t="s">
@@ -9546,7 +9117,7 @@
         <v>124</v>
       </c>
       <c r="AE57" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF57" s="18" t="s">
         <v>124</v>
@@ -9564,13 +9135,13 @@
         <v>124</v>
       </c>
       <c r="AK57" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL57" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM57" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN57" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9594,16 +9165,16 @@
         <v>123</v>
       </c>
       <c r="H58" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J58" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K58" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L58" t="s">
-        <v>313</v>
+        <v>148</v>
       </c>
       <c r="M58" t="s">
         <v>149</v>
@@ -9612,7 +9183,7 @@
         <v>134</v>
       </c>
       <c r="O58" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P58"/>
       <c r="Q58" s="18" t="s">
@@ -9648,31 +9219,31 @@
         <v>124</v>
       </c>
       <c r="AE58" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF58" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG58" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH58" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI58" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ58" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK58" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL58" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM58" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN58" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9699,16 +9270,16 @@
         <v>145</v>
       </c>
       <c r="J59" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K59" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L59" t="s">
-        <v>324</v>
+        <v>148</v>
       </c>
       <c r="M59" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N59" s="17" t="s">
         <v>134</v>
@@ -9768,13 +9339,13 @@
         <v>124</v>
       </c>
       <c r="AK59" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL59" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM59" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN59" s="18" t="str">
         <f t="shared" si="0"/>
@@ -9807,16 +9378,16 @@
         <v>158</v>
       </c>
       <c r="L60" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="M60" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N60" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O60" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P60"/>
       <c r="Q60" s="18" t="s">
@@ -9846,7 +9417,7 @@
         <v>124</v>
       </c>
       <c r="AC60" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD60" s="18" t="s">
         <v>124</v>
@@ -9858,7 +9429,7 @@
         <v>124</v>
       </c>
       <c r="AG60" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH60" s="18" t="s">
         <v>124</v>
@@ -9870,7 +9441,7 @@
         <v>124</v>
       </c>
       <c r="AK60" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL60" s="18" t="s">
         <v>124</v>
@@ -9903,22 +9474,22 @@
         <v>145</v>
       </c>
       <c r="J61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L61" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
       <c r="M61" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N61" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O61" s="18" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="P61"/>
       <c r="Q61" s="18" t="s">
@@ -9972,7 +9543,7 @@
         <v>124</v>
       </c>
       <c r="AK61" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL61" s="18" t="s">
         <v>124</v>
@@ -10005,22 +9576,22 @@
         <v>145</v>
       </c>
       <c r="J62" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="K62" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="L62" t="s">
-        <v>234</v>
+        <v>148</v>
       </c>
       <c r="M62" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N62" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O62" s="18" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="P62"/>
       <c r="Q62" s="18" t="s">
@@ -10050,31 +9621,31 @@
         <v>124</v>
       </c>
       <c r="AC62" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD62" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE62" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF62" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG62" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH62" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI62" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ62" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK62" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL62" s="18" t="s">
         <v>124</v>
@@ -10107,22 +9678,22 @@
         <v>145</v>
       </c>
       <c r="J63" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="K63" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="L63" t="s">
-        <v>236</v>
+        <v>148</v>
       </c>
       <c r="M63" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N63" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O63" s="18" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="P63"/>
       <c r="Q63" s="18" t="s">
@@ -10158,7 +9729,7 @@
         <v>124</v>
       </c>
       <c r="AE63" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF63" s="18" t="s">
         <v>124</v>
@@ -10176,7 +9747,7 @@
         <v>124</v>
       </c>
       <c r="AK63" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL63" s="18" t="s">
         <v>124</v>
@@ -10209,22 +9780,22 @@
         <v>145</v>
       </c>
       <c r="J64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K64" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L64" t="s">
-        <v>238</v>
+        <v>148</v>
       </c>
       <c r="M64" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N64" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O64" s="18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="P64"/>
       <c r="Q64" s="18" t="s">
@@ -10278,7 +9849,7 @@
         <v>124</v>
       </c>
       <c r="AK64" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL64" s="18" t="s">
         <v>124</v>
@@ -10311,22 +9882,22 @@
         <v>145</v>
       </c>
       <c r="J65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L65" t="s">
-        <v>240</v>
+        <v>148</v>
       </c>
       <c r="M65" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N65" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O65" s="18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="P65"/>
       <c r="Q65" s="18" t="s">
@@ -10362,7 +9933,7 @@
         <v>124</v>
       </c>
       <c r="AE65" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF65" s="18" t="s">
         <v>124</v>
@@ -10380,7 +9951,7 @@
         <v>124</v>
       </c>
       <c r="AK65" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL65" s="18" t="s">
         <v>124</v>
@@ -10413,22 +9984,22 @@
         <v>145</v>
       </c>
       <c r="J66" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L66" t="s">
-        <v>239</v>
+        <v>148</v>
       </c>
       <c r="M66" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N66" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O66" s="18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="P66"/>
       <c r="Q66" s="18" t="s">
@@ -10482,7 +10053,7 @@
         <v>124</v>
       </c>
       <c r="AK66" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL66" s="18" t="s">
         <v>124</v>
@@ -10515,22 +10086,22 @@
         <v>145</v>
       </c>
       <c r="J67" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="K67" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="L67" t="s">
-        <v>241</v>
+        <v>148</v>
       </c>
       <c r="M67" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N67" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O67" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P67"/>
       <c r="Q67" s="18" t="s">
@@ -10572,19 +10143,19 @@
         <v>124</v>
       </c>
       <c r="AG67" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH67" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI67" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ67" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK67" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL67" s="18" t="s">
         <v>124</v>
@@ -10617,22 +10188,22 @@
         <v>145</v>
       </c>
       <c r="J68" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="K68" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="L68" t="s">
-        <v>242</v>
+        <v>148</v>
       </c>
       <c r="M68" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N68" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O68" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P68"/>
       <c r="Q68" s="18" t="s">
@@ -10686,7 +10257,7 @@
         <v>124</v>
       </c>
       <c r="AK68" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL68" s="18" t="s">
         <v>124</v>
@@ -10716,25 +10287,25 @@
         <v>123</v>
       </c>
       <c r="H69" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J69" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K69" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L69" t="s">
-        <v>325</v>
+        <v>148</v>
       </c>
       <c r="M69" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N69" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O69" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P69"/>
       <c r="Q69" s="18" t="s">
@@ -10770,7 +10341,7 @@
         <v>124</v>
       </c>
       <c r="AE69" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF69" s="18" t="s">
         <v>124</v>
@@ -10788,13 +10359,13 @@
         <v>124</v>
       </c>
       <c r="AK69" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL69" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM69" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN69" s="18" t="str">
         <f t="shared" si="0"/>
@@ -10821,22 +10392,22 @@
         <v>145</v>
       </c>
       <c r="J70" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K70" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L70" t="s">
-        <v>244</v>
+        <v>148</v>
       </c>
       <c r="M70" t="s">
-        <v>245</v>
+        <v>186</v>
       </c>
       <c r="N70" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O70" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P70"/>
       <c r="Q70" s="18" t="s">
@@ -10866,31 +10437,31 @@
         <v>124</v>
       </c>
       <c r="AC70" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD70" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE70" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF70" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG70" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH70" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI70" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ70" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK70" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL70" s="18" t="s">
         <v>124</v>
@@ -10923,22 +10494,22 @@
         <v>145</v>
       </c>
       <c r="J71" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K71" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L71" t="s">
-        <v>243</v>
+        <v>148</v>
       </c>
       <c r="M71" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N71" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O71" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P71"/>
       <c r="Q71" s="18" t="s">
@@ -10968,31 +10539,31 @@
         <v>124</v>
       </c>
       <c r="AC71" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD71" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE71" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF71" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG71" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH71" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI71" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ71" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK71" s="18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="AL71" s="18" t="s">
         <v>124</v>
@@ -11022,25 +10593,25 @@
         <v>123</v>
       </c>
       <c r="H72" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J72" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K72" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L72" t="s">
-        <v>327</v>
+        <v>148</v>
       </c>
       <c r="M72" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N72" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O72" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P72"/>
       <c r="Q72" s="18" t="s">
@@ -11076,7 +10647,7 @@
         <v>124</v>
       </c>
       <c r="AE72" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF72" s="18" t="s">
         <v>124</v>
@@ -11094,13 +10665,13 @@
         <v>124</v>
       </c>
       <c r="AK72" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL72" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM72" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN72" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11124,25 +10695,25 @@
         <v>123</v>
       </c>
       <c r="H73" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J73" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K73" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L73" t="s">
-        <v>328</v>
+        <v>148</v>
       </c>
       <c r="M73" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N73" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O73" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P73"/>
       <c r="Q73" s="18" t="s">
@@ -11178,7 +10749,7 @@
         <v>124</v>
       </c>
       <c r="AE73" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF73" s="18" t="s">
         <v>124</v>
@@ -11196,13 +10767,13 @@
         <v>124</v>
       </c>
       <c r="AK73" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL73" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM73" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN73" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11226,25 +10797,25 @@
         <v>123</v>
       </c>
       <c r="H74" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J74" t="s">
-        <v>249</v>
+        <v>187</v>
       </c>
       <c r="K74" t="s">
-        <v>250</v>
+        <v>188</v>
       </c>
       <c r="L74" t="s">
-        <v>329</v>
+        <v>148</v>
       </c>
       <c r="M74" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N74" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O74" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P74"/>
       <c r="Q74" s="18" t="s">
@@ -11274,37 +10845,37 @@
         <v>124</v>
       </c>
       <c r="AC74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD74" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF74" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH74" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ74" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL74" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM74" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN74" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11331,16 +10902,16 @@
         <v>145</v>
       </c>
       <c r="J75" t="s">
-        <v>333</v>
+        <v>198</v>
       </c>
       <c r="K75" t="s">
-        <v>334</v>
+        <v>199</v>
       </c>
       <c r="L75" t="s">
-        <v>335</v>
+        <v>148</v>
       </c>
       <c r="M75" t="s">
-        <v>255</v>
+        <v>191</v>
       </c>
       <c r="N75" s="17" t="s">
         <v>134</v>
@@ -11400,13 +10971,13 @@
         <v>124</v>
       </c>
       <c r="AK75" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL75" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM75" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN75" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11433,22 +11004,22 @@
         <v>145</v>
       </c>
       <c r="J76" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="K76" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="L76" t="s">
-        <v>257</v>
+        <v>148</v>
       </c>
       <c r="M76" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N76" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O76" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P76"/>
       <c r="Q76" s="18" t="s">
@@ -11490,25 +11061,25 @@
         <v>124</v>
       </c>
       <c r="AG76" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH76" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI76" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ76" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK76" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL76" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM76" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN76" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11532,25 +11103,25 @@
         <v>123</v>
       </c>
       <c r="H77" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J77" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K77" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L77" t="s">
-        <v>337</v>
+        <v>148</v>
       </c>
       <c r="M77" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N77" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O77" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P77"/>
       <c r="Q77" s="18" t="s">
@@ -11586,7 +11157,7 @@
         <v>124</v>
       </c>
       <c r="AE77" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF77" s="18" t="s">
         <v>124</v>
@@ -11604,13 +11175,13 @@
         <v>124</v>
       </c>
       <c r="AK77" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL77" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM77" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN77" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11634,25 +11205,25 @@
         <v>123</v>
       </c>
       <c r="H78" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J78" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K78" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L78" t="s">
-        <v>339</v>
+        <v>148</v>
       </c>
       <c r="M78" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N78" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P78"/>
       <c r="Q78" s="18" t="s">
@@ -11688,7 +11259,7 @@
         <v>124</v>
       </c>
       <c r="AE78" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF78" s="18" t="s">
         <v>124</v>
@@ -11706,13 +11277,13 @@
         <v>124</v>
       </c>
       <c r="AK78" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL78" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM78" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN78" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11736,25 +11307,25 @@
         <v>123</v>
       </c>
       <c r="H79" t="s">
-        <v>282</v>
+        <v>197</v>
       </c>
       <c r="J79" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="K79" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="L79" t="s">
-        <v>341</v>
+        <v>148</v>
       </c>
       <c r="M79" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N79" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O79" s="18" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="P79"/>
       <c r="Q79" s="18" t="s">
@@ -11790,7 +11361,7 @@
         <v>124</v>
       </c>
       <c r="AE79" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF79" s="18" t="s">
         <v>124</v>
@@ -11808,13 +11379,13 @@
         <v>124</v>
       </c>
       <c r="AK79" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL79" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM79" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN79" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11841,22 +11412,22 @@
         <v>145</v>
       </c>
       <c r="J80" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K80" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L80" t="s">
-        <v>264</v>
+        <v>148</v>
       </c>
       <c r="M80" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N80" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O80" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P80"/>
       <c r="Q80" s="18" t="s">
@@ -11886,37 +11457,37 @@
         <v>124</v>
       </c>
       <c r="AC80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD80" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF80" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH80" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ80" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL80" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM80" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN80" s="18" t="str">
         <f t="shared" si="0"/>
@@ -11943,22 +11514,22 @@
         <v>145</v>
       </c>
       <c r="J81" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="K81" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="L81" t="s">
-        <v>265</v>
+        <v>148</v>
       </c>
       <c r="M81" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N81" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O81" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P81"/>
       <c r="Q81" s="18" t="s">
@@ -11988,37 +11559,37 @@
         <v>124</v>
       </c>
       <c r="AC81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD81" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF81" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH81" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ81" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL81" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM81" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN81" s="18" t="str">
         <f t="shared" si="0"/>
@@ -12042,25 +11613,25 @@
         <v>123</v>
       </c>
       <c r="H82" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J82" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="K82" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="L82" t="s">
-        <v>270</v>
+        <v>148</v>
       </c>
       <c r="M82" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
       <c r="N82" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O82" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P82"/>
       <c r="Q82" s="18" t="s">
@@ -12090,37 +11661,37 @@
         <v>124</v>
       </c>
       <c r="AC82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD82" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF82" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH82" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ82" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL82" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM82" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN82" s="18" t="str">
         <f t="shared" ref="AN82:AN91" si="1"><![CDATA[IF(OR(
@@ -12158,25 +11729,25 @@
         <v>123</v>
       </c>
       <c r="H83" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J83" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="K83" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="L83" t="s">
-        <v>342</v>
+        <v>148</v>
       </c>
       <c r="M83" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
       <c r="N83" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O83" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P83"/>
       <c r="Q83" s="18" t="s">
@@ -12206,37 +11777,37 @@
         <v>124</v>
       </c>
       <c r="AC83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD83" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF83" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH83" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ83" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL83" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM83" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN83" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12260,25 +11831,25 @@
         <v>123</v>
       </c>
       <c r="H84" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J84" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="K84" t="s">
-        <v>271</v>
+        <v>194</v>
       </c>
       <c r="L84" t="s">
-        <v>272</v>
+        <v>148</v>
       </c>
       <c r="M84" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N84" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O84" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P84"/>
       <c r="Q84" s="18" t="s">
@@ -12332,13 +11903,13 @@
         <v>124</v>
       </c>
       <c r="AK84" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL84" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM84" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN84" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12362,25 +11933,25 @@
         <v>123</v>
       </c>
       <c r="H85" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J85" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="K85" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="L85" t="s">
-        <v>277</v>
+        <v>148</v>
       </c>
       <c r="M85" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N85" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O85" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P85"/>
       <c r="Q85" s="18" t="s">
@@ -12434,13 +12005,13 @@
         <v>124</v>
       </c>
       <c r="AK85" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL85" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM85" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN85" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12464,25 +12035,25 @@
         <v>123</v>
       </c>
       <c r="H86" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J86" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="K86" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="L86" t="s">
-        <v>275</v>
+        <v>148</v>
       </c>
       <c r="M86" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N86" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O86" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P86"/>
       <c r="Q86" s="18" t="s">
@@ -12512,7 +12083,7 @@
         <v>124</v>
       </c>
       <c r="AC86" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD86" s="18" t="s">
         <v>124</v>
@@ -12524,25 +12095,25 @@
         <v>124</v>
       </c>
       <c r="AG86" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH86" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AI86" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AJ86" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AK86" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL86" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM86" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN86" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12566,25 +12137,25 @@
         <v>123</v>
       </c>
       <c r="H87" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J87" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="K87" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="L87" t="s">
-        <v>276</v>
+        <v>148</v>
       </c>
       <c r="M87" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N87" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O87" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P87"/>
       <c r="Q87" s="18" t="s">
@@ -12638,13 +12209,13 @@
         <v>124</v>
       </c>
       <c r="AK87" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL87" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM87" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN87" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12668,25 +12239,25 @@
         <v>123</v>
       </c>
       <c r="H88" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J88" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="K88" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="L88" t="s">
-        <v>274</v>
+        <v>148</v>
       </c>
       <c r="M88" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N88" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O88" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P88"/>
       <c r="Q88" s="18" t="s">
@@ -12740,13 +12311,13 @@
         <v>124</v>
       </c>
       <c r="AK88" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL88" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM88" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN88" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12770,25 +12341,25 @@
         <v>123</v>
       </c>
       <c r="H89" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J89" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="K89" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="L89" t="s">
-        <v>278</v>
+        <v>148</v>
       </c>
       <c r="M89" t="s">
-        <v>273</v>
+        <v>195</v>
       </c>
       <c r="N89" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O89" s="18" t="s">
-        <v>279</v>
+        <v>196</v>
       </c>
       <c r="P89"/>
       <c r="Q89" s="18" t="s">
@@ -12818,19 +12389,19 @@
         <v>124</v>
       </c>
       <c r="AC89" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD89" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AE89" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AF89" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AG89" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH89" s="18" t="s">
         <v>124</v>
@@ -12842,13 +12413,13 @@
         <v>124</v>
       </c>
       <c r="AK89" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL89" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM89" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN89" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12872,25 +12443,25 @@
         <v>123</v>
       </c>
       <c r="H90" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J90" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="K90" t="s">
-        <v>267</v>
+        <v>148</v>
       </c>
       <c r="L90" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M90" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
       <c r="N90" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O90" s="18" t="s">
-        <v>279</v>
+        <v>196</v>
       </c>
       <c r="P90"/>
       <c r="Q90" s="18" t="s">
@@ -12920,7 +12491,7 @@
         <v>124</v>
       </c>
       <c r="AC90" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AD90" s="18" t="s">
         <v>124</v>
@@ -12932,7 +12503,7 @@
         <v>124</v>
       </c>
       <c r="AG90" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AH90" s="18" t="s">
         <v>124</v>
@@ -12944,13 +12515,13 @@
         <v>124</v>
       </c>
       <c r="AK90" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL90" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM90" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN90" s="18" t="str">
         <f t="shared" si="1"/>
@@ -12974,25 +12545,25 @@
         <v>123</v>
       </c>
       <c r="H91" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="J91" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="K91" t="s">
-        <v>271</v>
+        <v>194</v>
       </c>
       <c r="L91" t="s">
-        <v>281</v>
+        <v>148</v>
       </c>
       <c r="M91" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="N91" s="17" t="s">
         <v>134</v>
       </c>
       <c r="O91" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="P91"/>
       <c r="Q91" s="18" t="s">
@@ -13046,13 +12617,13 @@
         <v>124</v>
       </c>
       <c r="AK91" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AL91" s="18" t="s">
         <v>124</v>
       </c>
       <c r="AM91" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="AN91" s="18" t="str">
         <f t="shared" si="1"/>

</xml_diff>